<commit_message>
add new post + update config
</commit_message>
<xml_diff>
--- a/docs/QuiFaitQuoi.xlsx
+++ b/docs/QuiFaitQuoi.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="90">
   <si>
     <t>Acteurs</t>
   </si>
@@ -204,16 +204,10 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Intégration/Dev de solutions IAM/SIEM</t>
-  </si>
-  <si>
     <t>Big Data</t>
   </si>
   <si>
     <t>SOFTEAM CADEXTAN</t>
-  </si>
-  <si>
-    <t>Formation dev securisé</t>
   </si>
   <si>
     <t>Sécurité systèmes embarqués
@@ -336,9 +330,6 @@
       </rPr>
       <t>Certification jeux en ligne (ARJEL)</t>
     </r>
-  </si>
-  <si>
-    <t>Cloud (IaaS, Paas, Saas)</t>
   </si>
   <si>
     <t>5 SOC à travers le monde</t>
@@ -514,12 +505,28 @@
     <t>Propose son propre antivirus
 Propose son propre SIEM (VigieSI)</t>
   </si>
+  <si>
+    <t>Cloud (IaaS, Paas, Saas) 
+MSSP (Managed Security Services Provider)</t>
+  </si>
+  <si>
+    <t>Développeurs sensibilisés sécu info</t>
+  </si>
+  <si>
+    <t>Assistance / conseil mise en conformité (LPM, ISO, PCI, ARJEL)</t>
+  </si>
+  <si>
+    <t>Assistance / conseil création SOC interne ou externalisation</t>
+  </si>
+  <si>
+    <t>Intégration/Dev de solutions IAM/SIEM (Offre Big Data SIEM)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -715,7 +722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -728,12 +735,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -751,17 +752,34 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -835,6 +853,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -869,6 +888,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1044,27 +1064,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="112" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="111.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1074,38 +1094,38 @@
       <c r="C1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="9"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="22"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="75">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1118,10 +1138,10 @@
         <v>29</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>25</v>
@@ -1133,8 +1153,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="60">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1147,21 +1167,21 @@
         <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>36</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="60">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1171,13 +1191,13 @@
         <v>43</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>30</v>
@@ -1189,8 +1209,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="45">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1200,13 +1220,13 @@
         <v>44</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>33</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>25</v>
@@ -1218,8 +1238,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1232,7 +1252,7 @@
         <v>47</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>48</v>
@@ -1245,8 +1265,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="60">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1259,10 +1279,10 @@
         <v>29</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>35</v>
@@ -1272,8 +1292,8 @@
       </c>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="45">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1283,10 +1303,10 @@
         <v>40</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
@@ -1297,11 +1317,11 @@
       </c>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="60">
-      <c r="A10" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="16" t="s">
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1311,73 +1331,73 @@
         <v>29</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G10" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>75</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>72</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="45">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="H11" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="105">
-      <c r="A12" s="13" t="s">
+    <row r="12" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>78</v>
+      <c r="E12" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>59</v>
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="30">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1388,13 +1408,13 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="17" t="s">
-        <v>87</v>
+      <c r="H13" s="15" t="s">
+        <v>84</v>
       </c>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="45">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1404,24 +1424,24 @@
         <v>24</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>64</v>
+        <v>82</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>62</v>
       </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="90">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1433,20 +1453,20 @@
       <c r="D15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>78</v>
+      <c r="E15" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="14" t="s">
-        <v>71</v>
+      <c r="H15" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="13" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1472,8 +1492,8 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1499,9 +1519,9 @@
       </c>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="13" t="s">
-        <v>54</v>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>19</v>
@@ -1526,40 +1546,50 @@
       </c>
       <c r="I18" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1"/>
-    <row r="21" spans="1:9">
-      <c r="A21" s="15" t="s">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A27" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1572,24 +1602,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>